<commit_message>
added the broken tag for all samples
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_paper_presentation\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB5898F-5C7A-4479-95DF-BF449CBE1879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F6E6A-6AD5-431C-B66B-B4A2B8715671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15372" yWindow="-13068" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
     <sheet name="Yellow 6 (broken)" sheetId="1" r:id="rId2"/>
     <sheet name="Green 6a (broken)" sheetId="4" r:id="rId3"/>
     <sheet name="Yellow 6a (broken)" sheetId="2" r:id="rId4"/>
-    <sheet name="Green 5" sheetId="3" r:id="rId5"/>
+    <sheet name="Green 5 (broken)" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="74">
   <si>
     <t>Y6</t>
   </si>
@@ -258,6 +258,10 @@
   </si>
   <si>
     <t>~250000</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>broken</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -4525,7 +4529,7 @@
   <dimension ref="A1:AK13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+      <selection activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4687,7 +4691,9 @@
         <v>8</v>
       </c>
       <c r="AI4" s="6"/>
-      <c r="AJ4" s="6"/>
+      <c r="AJ4" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="AK4" s="6"/>
     </row>
     <row r="5" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ignore the influence of pores for crack detection
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F6E6A-6AD5-431C-B66B-B4A2B8715671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3319F0-267E-4C50-B54D-7505CDE9358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,18 @@
     <sheet name="Yellow 6a (broken)" sheetId="2" r:id="rId4"/>
     <sheet name="Green 5 (broken)" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -270,9 +281,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,7 +409,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -758,9 +769,9 @@
       <selection pane="topRight" activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -805,7 +816,7 @@
       </c>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -853,7 +864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -915,7 +926,7 @@
       </c>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -977,7 +988,7 @@
       </c>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1039,7 +1050,7 @@
       </c>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1101,7 +1112,7 @@
       </c>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1163,7 +1174,7 @@
       </c>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1225,7 +1236,7 @@
       </c>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1287,7 +1298,7 @@
       </c>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1349,7 +1360,7 @@
       </c>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1413,7 +1424,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1475,7 +1486,7 @@
       </c>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1552,25 +1563,25 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.69921875" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" customWidth="1"/>
+    <col min="1" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="9.69921875" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
-    <col min="9" max="10" width="10.19921875" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="11.796875" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="10" width="10.25" customWidth="1"/>
+    <col min="11" max="11" width="10.625" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="10.25" customWidth="1"/>
+    <col min="14" max="14" width="11.375" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="1022" width="10.69921875" customWidth="1"/>
+    <col min="16" max="1022" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1588,7 +1599,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1604,7 +1615,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1661,7 +1672,7 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1718,7 +1729,7 @@
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1789,7 +1800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1860,7 +1871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1935,7 +1946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" s="4" customFormat="1">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -2012,7 +2023,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2083,7 +2094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2154,7 +2165,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="3" customFormat="1">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -2225,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" s="4" customFormat="1">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2438,7 +2449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2509,7 +2520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17">
         <v>13</v>
       </c>
@@ -2651,7 +2662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2722,7 +2733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2751,7 +2762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2768,7 +2779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2797,7 +2808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2826,7 +2837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2843,7 +2854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2928,21 +2939,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2999,7 +3010,7 @@
       </c>
       <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -3056,7 +3067,7 @@
       </c>
       <c r="AA4" s="6"/>
     </row>
-    <row r="5" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="4" customFormat="1">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -3157,19 +3168,19 @@
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16" width="10.69921875" customWidth="1"/>
-    <col min="17" max="17" width="12.19921875" customWidth="1"/>
-    <col min="18" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="16" width="10.75" customWidth="1"/>
+    <col min="17" max="17" width="12.25" customWidth="1"/>
+    <col min="18" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3230,7 +3241,7 @@
       </c>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3291,7 +3302,7 @@
       </c>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3368,7 +3379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3445,7 +3456,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3522,7 +3533,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3599,7 +3610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3676,7 +3687,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3753,7 +3764,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="4" customFormat="1">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -3830,7 +3841,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3907,7 +3918,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3984,7 +3995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>10</v>
       </c>
@@ -4061,7 +4072,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" s="3" customFormat="1">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -4138,7 +4149,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" s="3" customFormat="1">
       <c r="A16">
         <v>12</v>
       </c>
@@ -4179,7 +4190,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>13</v>
       </c>
@@ -4220,7 +4231,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -4255,7 +4266,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>15</v>
       </c>
@@ -4296,7 +4307,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>16</v>
       </c>
@@ -4343,7 +4354,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -4384,7 +4395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>18</v>
       </c>
@@ -4425,7 +4436,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>19</v>
       </c>
@@ -4472,7 +4483,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -4528,21 +4539,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AJ4" sqref="AJ4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -4619,7 +4631,7 @@
       </c>
       <c r="AK3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -4676,19 +4688,19 @@
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6" t="s">
@@ -4696,7 +4708,7 @@
       </c>
       <c r="AK4" s="6"/>
     </row>
-    <row r="5" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" s="4" customFormat="1">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -4800,366 +4812,375 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" spans="1:37">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="V6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6">
+        <v>646</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6">
+        <v>652</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB6">
+        <v>659</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD6">
+        <v>667</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>656</v>
+      </c>
+      <c r="AG6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH6">
+        <v>670</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="V7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>718</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z7">
+        <v>717</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB7">
+        <v>728</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD7">
+        <v>740</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF7">
+        <v>734</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH7">
+        <v>750</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" s="7" customFormat="1">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="P8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="7">
-        <v>1398</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="T6" s="7">
-        <v>1434</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="V6" s="7">
-        <v>1438</v>
-      </c>
-      <c r="W6" s="7" t="s">
+      <c r="R8" s="7">
+        <v>894</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" s="7">
+        <v>924</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8" s="7">
+        <v>933</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="7">
+        <v>889</v>
+      </c>
+      <c r="Y8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="X6" s="7">
-        <v>1398</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>1396</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB6" s="7">
-        <v>1406</v>
-      </c>
-      <c r="AC6" s="7" t="s">
+      <c r="Z8" s="7">
+        <v>889</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>898</v>
+      </c>
+      <c r="AC8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>909</v>
+      </c>
+      <c r="AE8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>894</v>
+      </c>
+      <c r="AG8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH8" s="7">
+        <v>908</v>
+      </c>
+      <c r="AI8" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" s="8" customFormat="1">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>929</v>
+      </c>
+      <c r="AC9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD9" s="8">
+        <v>931</v>
+      </c>
+      <c r="AE9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF9" s="8">
+        <v>928</v>
+      </c>
+      <c r="AG9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH9" s="8">
+        <v>940</v>
+      </c>
+      <c r="AI9" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" s="8" customFormat="1">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z10" s="8">
+        <v>949</v>
+      </c>
+      <c r="AA10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB10" s="8">
+        <v>954</v>
+      </c>
+      <c r="AC10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD10" s="8">
+        <v>955</v>
+      </c>
+      <c r="AE10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AD6" s="7">
-        <v>1419</v>
-      </c>
-      <c r="AE6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF6" s="7">
-        <v>1412</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH6" s="7">
-        <v>1422</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="V7" t="s">
-        <v>3</v>
-      </c>
-      <c r="W7" t="s">
-        <v>3</v>
-      </c>
-      <c r="X7">
-        <v>646</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z7">
-        <v>652</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB7">
-        <v>659</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD7">
-        <v>667</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF7" s="9">
-        <v>656</v>
-      </c>
-      <c r="AG7" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH7">
-        <v>670</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="V8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W8" t="s">
-        <v>3</v>
-      </c>
-      <c r="X8">
-        <v>718</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z8">
-        <v>717</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB8">
-        <v>728</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD8">
-        <v>740</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF8">
-        <v>734</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH8">
-        <v>750</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>5</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="R9" s="7">
-        <v>894</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="T9" s="7">
-        <v>924</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="V9" s="7">
-        <v>933</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X9" s="7">
-        <v>889</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z9" s="7">
-        <v>889</v>
-      </c>
-      <c r="AA9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB9" s="7">
-        <v>898</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD9" s="7">
-        <v>909</v>
-      </c>
-      <c r="AE9" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF9" s="7">
-        <v>894</v>
-      </c>
-      <c r="AG9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH9" s="7">
-        <v>908</v>
-      </c>
-      <c r="AI9" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Z10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB10" s="8">
-        <v>929</v>
-      </c>
-      <c r="AC10" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD10" s="8">
-        <v>931</v>
-      </c>
-      <c r="AE10" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="AF10" s="8">
-        <v>928</v>
+        <v>950</v>
       </c>
       <c r="AG10" s="8" t="s">
         <v>62</v>
       </c>
       <c r="AH10" s="8">
-        <v>940</v>
+        <v>964</v>
       </c>
       <c r="AI10" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="X11" s="8" t="s">
+    <row r="11" spans="1:37" s="8" customFormat="1">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="P11" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="Q11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="R11" s="8">
+        <v>1203</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="T11" s="8">
+        <v>1232</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" s="8">
+        <v>1233</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="X11" s="8">
+        <v>1205</v>
+      </c>
       <c r="Y11" s="8" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="Z11" s="8">
-        <v>949</v>
+        <v>1214</v>
       </c>
       <c r="AA11" s="8" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="AB11" s="8">
-        <v>954</v>
+        <v>1221</v>
       </c>
       <c r="AC11" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD11" s="8">
-        <v>955</v>
+        <v>1222</v>
       </c>
       <c r="AE11" s="8" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="AF11" s="8">
-        <v>950</v>
+        <v>1217</v>
       </c>
       <c r="AG11" s="8" t="s">
         <v>62</v>
       </c>
       <c r="AH11" s="8">
-        <v>964</v>
+        <v>1231</v>
       </c>
       <c r="AI11" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>6</v>
-      </c>
-      <c r="P12" s="8" t="s">
+    <row r="12" spans="1:37" s="7" customFormat="1">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="R12" s="8">
-        <v>1203</v>
-      </c>
-      <c r="S12" s="8" t="s">
+      <c r="R12" s="7">
+        <v>1398</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T12" s="7">
+        <v>1434</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="7">
+        <v>1438</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="X12" s="7">
+        <v>1398</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>1396</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>1406</v>
+      </c>
+      <c r="AC12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD12" s="7">
+        <v>1419</v>
+      </c>
+      <c r="AE12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF12" s="7">
+        <v>1412</v>
+      </c>
+      <c r="AG12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH12" s="7">
+        <v>1422</v>
+      </c>
+      <c r="AI12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="T12" s="8">
-        <v>1232</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="V12" s="8">
-        <v>1233</v>
-      </c>
-      <c r="W12" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="X12" s="8">
-        <v>1205</v>
-      </c>
-      <c r="Y12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z12" s="8">
-        <v>1214</v>
-      </c>
-      <c r="AA12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB12" s="8">
-        <v>1221</v>
-      </c>
-      <c r="AC12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD12" s="8">
-        <v>1222</v>
-      </c>
-      <c r="AE12" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF12" s="8">
-        <v>1217</v>
-      </c>
-      <c r="AG12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH12" s="8">
-        <v>1231</v>
-      </c>
-      <c r="AI12" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:37" s="8" customFormat="1">
+      <c r="A13">
+        <v>9</v>
+      </c>
       <c r="T13" s="8" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
no rotation and translation for cracks
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3319F0-267E-4C50-B54D-7505CDE9358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFA31D5-3616-4682-AD11-4D8618BBE918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="77">
   <si>
     <t>Y6</t>
   </si>
@@ -274,6 +274,15 @@
   <si>
     <t>broken</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fractured</t>
+  </si>
+  <si>
+    <t>Partly fractured</t>
+  </si>
+  <si>
+    <t>Totally fractured</t>
   </si>
 </sst>
 </file>
@@ -766,7 +775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R13" sqref="R13"/>
+      <selection pane="topRight" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1172,7 +1181,9 @@
         <f t="shared" si="0"/>
         <v>2.0482295482295481</v>
       </c>
-      <c r="W7" s="4"/>
+      <c r="W7" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="3">
@@ -1557,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AB24"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1581,7 +1592,7 @@
     <col min="16" max="1022" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1610,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:28">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1615,7 +1626,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1683,7 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1729,7 +1740,7 @@
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1800,7 +1811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1871,7 +1882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1946,7 +1957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="4" customFormat="1">
+    <row r="8" spans="1:28" s="4" customFormat="1">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -2022,8 +2033,11 @@
       <c r="AA8" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:27">
+      <c r="AB8" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2094,7 +2108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2165,7 +2179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="3" customFormat="1">
+    <row r="11" spans="1:28" s="3" customFormat="1">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -2236,7 +2250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="4" customFormat="1">
+    <row r="12" spans="1:28" s="4" customFormat="1">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -2306,8 +2320,11 @@
       <c r="AA12" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:27">
+      <c r="AB12" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2378,7 +2395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:28">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2449,7 +2466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:28">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2520,7 +2537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:28">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2937,10 +2954,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2948,12 +2965,12 @@
     <col min="1" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -3010,7 +3027,7 @@
       </c>
       <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -3067,7 +3084,7 @@
       </c>
       <c r="AA4" s="6"/>
     </row>
-    <row r="5" spans="1:27" s="4" customFormat="1">
+    <row r="5" spans="1:28" s="4" customFormat="1">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -3148,6 +3165,9 @@
       </c>
       <c r="AA5" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3162,10 +3182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AC24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AD32" sqref="AD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3456,741 +3476,561 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" s="3" customFormat="1">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>729</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>725</v>
-      </c>
-      <c r="K7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7">
-        <v>718</v>
-      </c>
-      <c r="M7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7">
-        <v>722</v>
-      </c>
-      <c r="O7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P7">
-        <v>697</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7">
-        <v>748</v>
-      </c>
-      <c r="S7" t="s">
-        <v>5</v>
-      </c>
-      <c r="T7">
-        <v>711</v>
-      </c>
-      <c r="U7" t="s">
-        <v>6</v>
-      </c>
-      <c r="V7">
-        <v>729</v>
-      </c>
-      <c r="W7" t="s">
-        <v>8</v>
-      </c>
-      <c r="X7">
-        <v>719</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z7">
-        <v>729</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB7">
-        <v>726</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>62</v>
+      <c r="R7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T7" s="3">
+        <v>516</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V7" s="3">
+        <v>523</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="X7" s="3">
+        <v>514</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>531</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>534</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="F8">
-        <v>804</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>817</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>824</v>
-      </c>
-      <c r="K8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8">
-        <v>824</v>
-      </c>
-      <c r="M8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8">
-        <v>829</v>
-      </c>
-      <c r="O8" t="s">
-        <v>8</v>
-      </c>
-      <c r="P8">
-        <v>780</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>4</v>
-      </c>
-      <c r="R8">
-        <v>844</v>
+      <c r="R8" t="s">
+        <v>66</v>
       </c>
       <c r="S8" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="T8">
-        <v>805</v>
+        <v>636</v>
       </c>
       <c r="U8" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="V8">
-        <v>815</v>
+        <v>644</v>
       </c>
       <c r="W8" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="X8">
-        <v>805</v>
+        <v>635</v>
       </c>
       <c r="Y8" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="Z8">
-        <v>816</v>
+        <v>644</v>
       </c>
       <c r="AA8" t="s">
         <v>5</v>
       </c>
       <c r="AB8">
-        <v>825</v>
+        <v>654</v>
       </c>
       <c r="AC8" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>935</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9">
-        <v>942</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <v>940</v>
-      </c>
-      <c r="M9" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9">
-        <v>938</v>
-      </c>
-      <c r="O9" t="s">
-        <v>8</v>
-      </c>
-      <c r="P9">
-        <v>889</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>11</v>
-      </c>
-      <c r="R9">
-        <v>949</v>
-      </c>
-      <c r="S9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T9">
-        <v>918</v>
+      <c r="T9" t="s">
+        <v>66</v>
       </c>
       <c r="U9" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="V9">
-        <v>926</v>
+        <v>699</v>
       </c>
       <c r="W9" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="X9">
-        <v>916</v>
+        <v>690</v>
       </c>
       <c r="Y9" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="Z9">
-        <v>932</v>
+        <v>705</v>
       </c>
       <c r="AA9" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="AB9">
-        <v>933</v>
+        <v>710</v>
       </c>
       <c r="AC9" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="F10">
-        <v>1013</v>
+      <c r="F10" t="s">
+        <v>3</v>
       </c>
       <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>729</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>725</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>718</v>
+      </c>
+      <c r="M10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10">
+        <v>722</v>
+      </c>
+      <c r="O10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>697</v>
+      </c>
+      <c r="Q10" t="s">
         <v>12</v>
       </c>
-      <c r="H10">
-        <v>1040</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10">
-        <v>1037</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="R10">
+        <v>748</v>
+      </c>
+      <c r="S10" t="s">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>711</v>
+      </c>
+      <c r="U10" t="s">
+        <v>6</v>
+      </c>
+      <c r="V10">
+        <v>729</v>
+      </c>
+      <c r="W10" t="s">
+        <v>8</v>
+      </c>
+      <c r="X10">
+        <v>719</v>
+      </c>
+      <c r="Y10" t="s">
         <v>12</v>
       </c>
-      <c r="L10">
-        <v>1030</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="Z10">
+        <v>729</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB10">
+        <v>726</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>804</v>
+      </c>
+      <c r="G11" t="s">
         <v>5</v>
       </c>
-      <c r="N10">
-        <v>1030</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="H11">
+        <v>817</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>824</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>824</v>
+      </c>
+      <c r="M11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>829</v>
+      </c>
+      <c r="O11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>780</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>844</v>
+      </c>
+      <c r="S11" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11">
+        <v>805</v>
+      </c>
+      <c r="U11" t="s">
+        <v>29</v>
+      </c>
+      <c r="V11">
+        <v>815</v>
+      </c>
+      <c r="W11" t="s">
         <v>9</v>
       </c>
-      <c r="P10">
-        <v>995</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10">
-        <v>1049</v>
-      </c>
-      <c r="S10" t="s">
-        <v>4</v>
-      </c>
-      <c r="T10">
-        <v>1019</v>
-      </c>
-      <c r="U10" t="s">
-        <v>11</v>
-      </c>
-      <c r="V10">
-        <v>1034</v>
-      </c>
-      <c r="W10" t="s">
-        <v>6</v>
-      </c>
-      <c r="X10">
-        <v>1024</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z10">
-        <v>1038</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB10">
-        <v>1031</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" s="4" customFormat="1">
-      <c r="A11" s="4">
-        <v>7</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1119</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1149</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="4">
-        <v>1144</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="4">
-        <v>1137</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="4">
-        <v>1139</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1111</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="4">
-        <v>1163</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T11" s="4">
-        <v>1127</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V11" s="4">
-        <v>1143</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="X11" s="4">
-        <v>1133</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z11" s="4">
-        <v>1142</v>
-      </c>
-      <c r="AA11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB11" s="4">
-        <v>1139</v>
-      </c>
-      <c r="AC11" s="4" t="s">
-        <v>62</v>
+      <c r="X11">
+        <v>805</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z11">
+        <v>816</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB11">
+        <v>825</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>1169</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12">
-        <v>1172</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="R12" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T12">
+        <v>889</v>
+      </c>
+      <c r="U12" t="s">
+        <v>69</v>
+      </c>
+      <c r="V12">
+        <v>896</v>
+      </c>
+      <c r="W12" t="s">
+        <v>58</v>
+      </c>
+      <c r="X12">
+        <v>887</v>
+      </c>
+      <c r="Y12" t="s">
         <v>5</v>
       </c>
-      <c r="L12">
-        <v>1174</v>
-      </c>
-      <c r="M12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12">
-        <v>1181</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="Z12">
+        <v>905</v>
+      </c>
+      <c r="AA12" t="s">
         <v>6</v>
       </c>
-      <c r="P12">
-        <v>1131</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>4</v>
-      </c>
-      <c r="R12">
-        <v>1194</v>
-      </c>
-      <c r="S12" t="s">
-        <v>8</v>
-      </c>
-      <c r="T12">
-        <v>1156</v>
-      </c>
-      <c r="U12" t="s">
-        <v>10</v>
-      </c>
-      <c r="V12">
-        <v>1164</v>
-      </c>
-      <c r="W12" t="s">
-        <v>9</v>
-      </c>
-      <c r="X12">
-        <v>1154</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z12">
-        <v>1163</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>5</v>
-      </c>
       <c r="AB12">
-        <v>1173</v>
+        <v>907</v>
       </c>
       <c r="AC12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="F13">
-        <v>1279</v>
+      <c r="F13" t="s">
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>1291</v>
+        <v>935</v>
       </c>
       <c r="I13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J13">
-        <v>1299</v>
+        <v>942</v>
       </c>
       <c r="K13" t="s">
         <v>6</v>
       </c>
       <c r="L13">
-        <v>1297</v>
+        <v>940</v>
       </c>
       <c r="M13" t="s">
         <v>9</v>
       </c>
       <c r="N13">
-        <v>1291</v>
+        <v>938</v>
       </c>
       <c r="O13" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="3">
-        <v>1245</v>
-      </c>
-      <c r="Q13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P13">
+        <v>889</v>
+      </c>
+      <c r="Q13" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="3">
-        <v>1297</v>
-      </c>
-      <c r="S13" s="3" t="s">
+      <c r="R13">
+        <v>949</v>
+      </c>
+      <c r="S13" t="s">
         <v>10</v>
       </c>
       <c r="T13">
-        <v>1273</v>
+        <v>918</v>
       </c>
       <c r="U13" t="s">
         <v>9</v>
       </c>
       <c r="V13">
-        <v>1279</v>
+        <v>926</v>
       </c>
       <c r="W13" t="s">
         <v>4</v>
       </c>
       <c r="X13">
-        <v>1271</v>
+        <v>916</v>
       </c>
       <c r="Y13" t="s">
         <v>5</v>
       </c>
       <c r="Z13">
-        <v>1286</v>
+        <v>932</v>
       </c>
       <c r="AA13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="AB13">
-        <v>1291</v>
+        <v>933</v>
       </c>
       <c r="AC13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="F14" t="s">
-        <v>3</v>
+      <c r="F14">
+        <v>1013</v>
       </c>
       <c r="G14" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H14">
-        <v>1390</v>
+        <v>1040</v>
       </c>
       <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>1037</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>1030</v>
+      </c>
+      <c r="M14" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>1030</v>
+      </c>
+      <c r="O14" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14">
+        <v>995</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <v>1049</v>
+      </c>
+      <c r="S14" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14">
+        <v>1019</v>
+      </c>
+      <c r="U14" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14">
+        <v>1034</v>
+      </c>
+      <c r="W14" t="s">
         <v>6</v>
       </c>
-      <c r="J14">
-        <v>1383</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="X14">
+        <v>1024</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z14">
+        <v>1038</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB14">
+        <v>1031</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="P15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>66</v>
+      </c>
+      <c r="R15">
+        <v>1196</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15">
+        <v>1071</v>
+      </c>
+      <c r="U15" t="s">
+        <v>62</v>
+      </c>
+      <c r="V15">
+        <v>1084</v>
+      </c>
+      <c r="W15" t="s">
+        <v>63</v>
+      </c>
+      <c r="X15">
+        <v>1074</v>
+      </c>
+      <c r="Y15" t="s">
         <v>9</v>
       </c>
-      <c r="L14">
-        <v>1380</v>
-      </c>
-      <c r="M14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N14">
-        <v>1383</v>
-      </c>
-      <c r="O14" t="s">
-        <v>5</v>
-      </c>
-      <c r="P14" s="3">
-        <v>1356</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R14" s="3">
-        <v>1411</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T14">
-        <v>1370</v>
-      </c>
-      <c r="U14" t="s">
-        <v>6</v>
-      </c>
-      <c r="V14">
-        <v>1388</v>
-      </c>
-      <c r="W14" t="s">
-        <v>8</v>
-      </c>
-      <c r="X14">
-        <v>1376</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z14">
-        <v>1384</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB14">
-        <v>1384</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" s="3" customFormat="1">
-      <c r="A15" s="3">
-        <v>11</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1400</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1428</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="3">
-        <v>1426</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="3">
-        <v>1417</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N15" s="3">
-        <v>1414</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P15" s="3">
-        <v>1387</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R15" s="3">
-        <v>1433</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="3">
-        <v>1407</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V15" s="3">
-        <v>1422</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X15" s="3">
-        <v>1410</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z15" s="3">
-        <v>1427</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB15" s="3">
-        <v>1421</v>
-      </c>
-      <c r="AC15" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" s="3" customFormat="1">
+      <c r="Z15">
+        <v>1081</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB15">
+        <v>1090</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="R16" s="3" t="s">
+      <c r="R16" t="s">
         <v>66</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="T16" s="3">
-        <v>516</v>
-      </c>
-      <c r="U16" s="3" t="s">
+      <c r="T16">
+        <v>1075</v>
+      </c>
+      <c r="U16" t="s">
+        <v>59</v>
+      </c>
+      <c r="V16">
+        <v>1082</v>
+      </c>
+      <c r="W16" t="s">
         <v>69</v>
       </c>
-      <c r="V16" s="3">
-        <v>523</v>
-      </c>
-      <c r="W16" s="3" t="s">
+      <c r="X16">
+        <v>1072</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16">
+        <v>1085</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB16">
+        <v>1094</v>
+      </c>
+      <c r="AC16" t="s">
         <v>58</v>
       </c>
-      <c r="X16" s="3">
-        <v>514</v>
-      </c>
-      <c r="Y16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>531</v>
-      </c>
-      <c r="AA16" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB16" s="3">
-        <v>534</v>
-      </c>
-      <c r="AC16" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29">
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17">
         <v>13</v>
       </c>
@@ -4200,328 +4040,511 @@
       <c r="S17" t="s">
         <v>66</v>
       </c>
-      <c r="T17">
-        <v>636</v>
+      <c r="T17" t="s">
+        <v>66</v>
       </c>
       <c r="U17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="V17">
-        <v>644</v>
+        <v>1129</v>
       </c>
       <c r="W17" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="X17">
-        <v>635</v>
+        <v>1121</v>
       </c>
       <c r="Y17" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="Z17">
-        <v>644</v>
+        <v>1135</v>
       </c>
       <c r="AA17" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="AB17">
-        <v>654</v>
+        <v>1142</v>
       </c>
       <c r="AC17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29">
-      <c r="A18" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" s="4" customFormat="1">
+      <c r="A18">
         <v>14</v>
       </c>
-      <c r="T18" t="s">
-        <v>66</v>
-      </c>
-      <c r="U18" t="s">
-        <v>66</v>
-      </c>
-      <c r="V18">
-        <v>699</v>
-      </c>
-      <c r="W18" t="s">
-        <v>69</v>
-      </c>
-      <c r="X18">
-        <v>690</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z18">
-        <v>705</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB18">
-        <v>710</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29">
+      <c r="F18" s="4">
+        <v>1119</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1149</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1144</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1137</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1139</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1111</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R18" s="4">
+        <v>1163</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" s="4">
+        <v>1127</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" s="4">
+        <v>1143</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X18" s="4">
+        <v>1133</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>1142</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB18" s="4">
+        <v>1139</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD18" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="R19" t="s">
-        <v>66</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>66</v>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>1169</v>
+      </c>
+      <c r="I19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>1172</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>1174</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>1181</v>
+      </c>
+      <c r="O19" t="s">
+        <v>6</v>
+      </c>
+      <c r="P19">
+        <v>1131</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19">
+        <v>1194</v>
+      </c>
+      <c r="S19" t="s">
+        <v>8</v>
       </c>
       <c r="T19">
-        <v>889</v>
+        <v>1156</v>
       </c>
       <c r="U19" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19">
+        <v>1164</v>
+      </c>
+      <c r="W19" t="s">
+        <v>9</v>
+      </c>
+      <c r="X19">
+        <v>1154</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z19">
+        <v>1163</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB19">
+        <v>1173</v>
+      </c>
+      <c r="AC19" t="s">
         <v>69</v>
       </c>
-      <c r="V19">
-        <v>896</v>
-      </c>
-      <c r="W19" t="s">
-        <v>58</v>
-      </c>
-      <c r="X19">
-        <v>887</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z19">
-        <v>905</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB19">
-        <v>907</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29">
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="P20" t="s">
+      <c r="F20">
+        <v>1279</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>1291</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>1299</v>
+      </c>
+      <c r="K20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <v>1297</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20">
+        <v>1291</v>
+      </c>
+      <c r="O20" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="3">
+        <v>1245</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1297</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20">
+        <v>1273</v>
+      </c>
+      <c r="U20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V20">
+        <v>1279</v>
+      </c>
+      <c r="W20" t="s">
+        <v>4</v>
+      </c>
+      <c r="X20">
+        <v>1271</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z20">
+        <v>1286</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB20">
+        <v>1291</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="P21" t="s">
         <v>66</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q21" t="s">
         <v>66</v>
       </c>
-      <c r="R20">
-        <v>1196</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="T20">
-        <v>1071</v>
-      </c>
-      <c r="U20" t="s">
-        <v>62</v>
-      </c>
-      <c r="V20">
-        <v>1084</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="R21">
+        <v>1317</v>
+      </c>
+      <c r="S21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="X20">
-        <v>1074</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z20">
-        <v>1081</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB20">
-        <v>1090</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29">
-      <c r="A21" s="3">
-        <v>17</v>
-      </c>
-      <c r="R21" t="s">
-        <v>66</v>
-      </c>
-      <c r="S21" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="T21">
-        <v>1075</v>
+        <v>1289</v>
       </c>
       <c r="U21" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="V21">
-        <v>1082</v>
+        <v>1296</v>
       </c>
       <c r="W21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="X21">
-        <v>1072</v>
+        <v>1287</v>
       </c>
       <c r="Y21" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="Z21">
-        <v>1085</v>
+        <v>1303</v>
       </c>
       <c r="AA21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="AB21">
-        <v>1094</v>
+        <v>1306</v>
       </c>
       <c r="AC21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="R22" t="s">
-        <v>66</v>
-      </c>
-      <c r="S22" t="s">
-        <v>66</v>
-      </c>
-      <c r="T22" t="s">
-        <v>66</v>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>1390</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22">
+        <v>1383</v>
+      </c>
+      <c r="K22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>1380</v>
+      </c>
+      <c r="M22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>1383</v>
+      </c>
+      <c r="O22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="3">
+        <v>1356</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R22" s="3">
+        <v>1411</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T22">
+        <v>1370</v>
       </c>
       <c r="U22" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="V22">
-        <v>1129</v>
+        <v>1388</v>
       </c>
       <c r="W22" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="X22">
-        <v>1121</v>
+        <v>1376</v>
       </c>
       <c r="Y22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Z22">
-        <v>1135</v>
+        <v>1384</v>
       </c>
       <c r="AA22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB22">
-        <v>1142</v>
+        <v>1384</v>
       </c>
       <c r="AC22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>66</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="S23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R23">
-        <v>1317</v>
-      </c>
-      <c r="S23" s="3" t="s">
+      <c r="T23">
+        <v>1386</v>
+      </c>
+      <c r="U23" t="s">
+        <v>61</v>
+      </c>
+      <c r="V23">
+        <v>1402</v>
+      </c>
+      <c r="W23" t="s">
+        <v>62</v>
+      </c>
+      <c r="X23">
+        <v>1387</v>
+      </c>
+      <c r="Y23" t="s">
         <v>63</v>
       </c>
-      <c r="T23">
-        <v>1289</v>
-      </c>
-      <c r="U23" t="s">
-        <v>69</v>
-      </c>
-      <c r="V23">
-        <v>1296</v>
-      </c>
-      <c r="W23" t="s">
-        <v>58</v>
-      </c>
-      <c r="X23">
-        <v>1287</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>58</v>
-      </c>
       <c r="Z23">
-        <v>1303</v>
+        <v>1398</v>
       </c>
       <c r="AA23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB23">
+        <v>1399</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="3" customFormat="1">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1400</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1428</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1426</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1417</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1414</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" s="3">
+        <v>1387</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="3">
+        <v>1433</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1407</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V24" s="3">
+        <v>1422</v>
+      </c>
+      <c r="W24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB23">
-        <v>1306</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29">
-      <c r="A24" s="3">
-        <v>20</v>
-      </c>
-      <c r="R24" t="s">
-        <v>66</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="T24">
-        <v>1386</v>
-      </c>
-      <c r="U24" t="s">
+      <c r="X24" s="3">
+        <v>1410</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>1427</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>1421</v>
+      </c>
+      <c r="AC24" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="V24">
-        <v>1402</v>
-      </c>
-      <c r="W24" t="s">
-        <v>62</v>
-      </c>
-      <c r="X24">
-        <v>1387</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z24">
-        <v>1398</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB24">
-        <v>1399</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4539,9 +4562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S16" sqref="S16"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5176,6 +5199,9 @@
       <c r="AI12" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="AJ12" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="1:37" s="8" customFormat="1">
       <c r="A13">

</xml_diff>

<commit_message>
modified the crack site of AMY6a
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFA31D5-3616-4682-AD11-4D8618BBE918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D350103C-02A8-4A40-8B1B-C0AFFBBD22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="78">
   <si>
     <t>Y6</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Totally fractured</t>
+  </si>
+  <si>
+    <t>Same height</t>
   </si>
 </sst>
 </file>
@@ -352,7 +355,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +372,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF7F"/>
         <bgColor rgb="FF00FF7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -422,7 +437,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -451,6 +466,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2956,7 +2989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
@@ -3182,25 +3215,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD24"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AD32" sqref="AD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16" width="10.75" customWidth="1"/>
     <col min="17" max="17" width="12.25" customWidth="1"/>
-    <col min="18" max="1024" width="10.75" customWidth="1"/>
+    <col min="18" max="29" width="10.75" customWidth="1"/>
+    <col min="30" max="30" width="11.875" customWidth="1"/>
+    <col min="31" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3261,7 +3297,7 @@
       </c>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3322,7 +3358,7 @@
       </c>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3399,7 +3435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3476,7 +3512,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="3" customFormat="1">
+    <row r="7" spans="1:30" s="3" customFormat="1">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3517,7 +3553,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3558,7 +3594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3593,7 +3629,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3670,7 +3706,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3747,7 +3783,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3788,7 +3824,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3865,7 +3901,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3942,216 +3978,224 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
-      <c r="A15">
+    <row r="15" spans="1:30" s="10" customFormat="1">
+      <c r="A15" s="10">
         <v>11</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="10">
         <v>1196</v>
       </c>
-      <c r="S15" s="3" t="s">
+      <c r="S15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="10">
         <v>1071</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="10">
         <v>1084</v>
       </c>
-      <c r="W15" t="s">
+      <c r="W15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="10">
         <v>1074</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Y15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="10">
         <v>1081</v>
       </c>
-      <c r="AA15" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB15">
+      <c r="AA15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="10">
         <v>1090</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AC15" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:29">
-      <c r="A16">
+      <c r="AD15" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="10" customFormat="1">
+      <c r="A16" s="10">
         <v>12</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="S16" s="3" t="s">
+      <c r="S16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="10">
         <v>1075</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="10">
         <v>1082</v>
       </c>
-      <c r="W16" t="s">
+      <c r="W16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="10">
         <v>1072</v>
       </c>
-      <c r="Y16" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z16">
+      <c r="Y16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="10">
         <v>1085</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AA16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AB16">
+      <c r="AB16" s="10">
         <v>1094</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AC16" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:30">
-      <c r="A17">
+      <c r="AD16" s="12"/>
+    </row>
+    <row r="17" spans="1:31" s="13" customFormat="1">
+      <c r="A17" s="13">
         <v>13</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="13">
         <v>1129</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W17" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="13">
         <v>1121</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Y17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="13">
         <v>1135</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" s="13">
         <v>1142</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AC17" s="13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" s="4" customFormat="1">
-      <c r="A18">
+      <c r="AD17" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" s="15" customFormat="1">
+      <c r="A18" s="13">
         <v>14</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="15">
         <v>1119</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="15">
         <v>1149</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="15">
         <v>1144</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="15">
         <v>1137</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="15">
         <v>1139</v>
       </c>
-      <c r="O18" s="4" t="s">
+      <c r="O18" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="15">
         <v>1111</v>
       </c>
-      <c r="Q18" s="4" t="s">
+      <c r="Q18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18" s="15">
         <v>1163</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="S18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T18" s="15">
         <v>1127</v>
       </c>
-      <c r="U18" s="4" t="s">
+      <c r="U18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="V18" s="4">
+      <c r="V18" s="15">
         <v>1143</v>
       </c>
-      <c r="W18" s="4" t="s">
+      <c r="W18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="X18" s="4">
+      <c r="X18" s="15">
         <v>1133</v>
       </c>
-      <c r="Y18" s="4" t="s">
+      <c r="Y18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="Z18" s="4">
+      <c r="Z18" s="15">
         <v>1142</v>
       </c>
-      <c r="AA18" s="4" t="s">
+      <c r="AA18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AB18" s="4">
+      <c r="AB18" s="15">
         <v>1139</v>
       </c>
-      <c r="AC18" s="4" t="s">
+      <c r="AC18" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="AD18" s="4" t="s">
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:31">
       <c r="A19">
         <v>15</v>
       </c>
@@ -4228,7 +4272,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:31">
       <c r="A20">
         <v>16</v>
       </c>
@@ -4305,7 +4349,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:31">
       <c r="A21">
         <v>17</v>
       </c>
@@ -4352,7 +4396,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:31">
       <c r="A22">
         <v>18</v>
       </c>
@@ -4429,7 +4473,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:31">
       <c r="A23">
         <v>19</v>
       </c>
@@ -4470,7 +4514,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="3" customFormat="1">
+    <row r="24" spans="1:31" s="3" customFormat="1">
       <c r="A24">
         <v>20</v>
       </c>
@@ -4548,6 +4592,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="AD17:AD18"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39416666666666667" bottom="0.39416666666666667" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified the crack order for Yellow6
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D350103C-02A8-4A40-8B1B-C0AFFBBD22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FBCB9F-D6F9-411D-8C70-795DCD608F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -474,17 +474,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1603,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2074,357 +2074,258 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>718</v>
-      </c>
-      <c r="M9" t="s">
-        <v>12</v>
-      </c>
-      <c r="N9">
-        <v>719</v>
-      </c>
-      <c r="O9" t="s">
-        <v>9</v>
-      </c>
-      <c r="P9">
-        <v>789</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>8</v>
-      </c>
-      <c r="R9">
-        <v>707</v>
-      </c>
-      <c r="S9" t="s">
-        <v>8</v>
-      </c>
-      <c r="T9">
-        <v>715</v>
+      <c r="T9" t="s">
+        <v>66</v>
       </c>
       <c r="U9" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="V9">
-        <v>726</v>
+        <v>629</v>
       </c>
       <c r="W9" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="X9">
-        <v>702</v>
+        <v>595</v>
       </c>
       <c r="Y9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z9">
-        <v>725</v>
+        <v>624</v>
       </c>
       <c r="AA9" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:28">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="F10">
-        <v>806</v>
+      <c r="F10" t="s">
+        <v>3</v>
       </c>
       <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>718</v>
+      </c>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10">
+        <v>719</v>
+      </c>
+      <c r="O10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>789</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>707</v>
+      </c>
+      <c r="S10" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <v>715</v>
+      </c>
+      <c r="U10" t="s">
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <v>726</v>
+      </c>
+      <c r="W10" t="s">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>702</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z10">
+        <v>725</v>
+      </c>
+      <c r="AA10" t="s">
         <v>10</v>
       </c>
-      <c r="H10">
-        <v>828</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10">
-        <v>836</v>
-      </c>
-      <c r="K10" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10">
-        <v>825</v>
-      </c>
-      <c r="M10" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10">
-        <v>823</v>
-      </c>
-      <c r="O10" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10">
-        <v>885</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>4</v>
-      </c>
-      <c r="R10">
-        <v>811</v>
-      </c>
-      <c r="S10" t="s">
-        <v>4</v>
-      </c>
-      <c r="T10">
-        <v>827</v>
-      </c>
-      <c r="U10" t="s">
-        <v>6</v>
-      </c>
-      <c r="V10">
-        <v>832</v>
-      </c>
-      <c r="W10" t="s">
-        <v>8</v>
-      </c>
-      <c r="X10">
-        <v>800</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z10">
-        <v>826</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="3" customFormat="1">
+    </row>
+    <row r="11" spans="1:28">
       <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="3">
-        <v>846</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="3">
-        <v>861</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="3">
-        <v>842</v>
-      </c>
-      <c r="M11" s="3" t="s">
+      <c r="X11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z11">
+        <v>824</v>
+      </c>
+      <c r="AA11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="3">
-        <v>845</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P11" s="3">
-        <v>914</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R11" s="3">
-        <v>834</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T11" s="3">
-        <v>839</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="V11" s="3">
-        <v>849</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="X11" s="3">
-        <v>824</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z11" s="3">
-        <v>846</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" s="4" customFormat="1">
+    </row>
+    <row r="12" spans="1:28">
       <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="F12" s="5">
-        <v>853</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="F12">
+        <v>806</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>828</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>836</v>
+      </c>
+      <c r="K12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>825</v>
+      </c>
+      <c r="M12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>823</v>
+      </c>
+      <c r="O12" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="4">
-        <v>870</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="P12">
+        <v>885</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <v>811</v>
+      </c>
+      <c r="S12" t="s">
+        <v>4</v>
+      </c>
+      <c r="T12">
+        <v>827</v>
+      </c>
+      <c r="U12" t="s">
+        <v>6</v>
+      </c>
+      <c r="V12">
+        <v>832</v>
+      </c>
+      <c r="W12" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12">
+        <v>800</v>
+      </c>
+      <c r="Y12" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="4">
-        <v>883</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="4">
-        <v>867</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="4">
-        <v>868</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P12" s="4">
-        <v>937</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R12" s="4">
-        <v>856</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T12" s="4">
-        <v>865</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="V12" s="4">
-        <v>872</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="X12" s="4">
-        <v>844</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z12" s="4">
-        <v>863</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28">
+      <c r="Z12">
+        <v>826</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="3" customFormat="1">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13">
-        <v>923</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>846</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="3">
+        <v>861</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="3">
+        <v>842</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N13">
-        <v>924</v>
-      </c>
-      <c r="O13" t="s">
-        <v>9</v>
-      </c>
-      <c r="P13">
-        <v>992</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="N13" s="3">
+        <v>845</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="3">
+        <v>914</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="3">
+        <v>834</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="3">
+        <v>839</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="3">
+        <v>849</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X13" s="3">
+        <v>824</v>
+      </c>
+      <c r="Y13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R13">
-        <v>909</v>
-      </c>
-      <c r="S13" t="s">
-        <v>8</v>
-      </c>
-      <c r="T13">
-        <v>919</v>
-      </c>
-      <c r="U13" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13">
-        <v>928</v>
-      </c>
-      <c r="W13" t="s">
-        <v>5</v>
-      </c>
-      <c r="X13">
-        <v>904</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z13">
-        <v>927</v>
-      </c>
-      <c r="AA13" t="s">
+      <c r="Z13" s="3">
+        <v>846</v>
+      </c>
+      <c r="AA13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2432,210 +2333,171 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="F14">
-        <v>960</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="T14" t="s">
+        <v>66</v>
+      </c>
+      <c r="U14" t="s">
+        <v>66</v>
+      </c>
+      <c r="V14">
+        <v>857</v>
+      </c>
+      <c r="W14" t="s">
+        <v>68</v>
+      </c>
+      <c r="X14">
+        <v>826</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z14">
+        <v>847</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="4" customFormat="1">
+      <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="H14">
-        <v>977</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="F15" s="5">
+        <v>853</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="4">
+        <v>870</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J14">
-        <v>993</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="J15" s="4">
+        <v>883</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="4">
+        <v>867</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" s="4">
+        <v>868</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="4">
+        <v>937</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" s="4">
+        <v>856</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" s="4">
+        <v>865</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" s="4">
+        <v>872</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X15" s="4">
+        <v>844</v>
+      </c>
+      <c r="Y15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L14">
-        <v>970</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="Z15" s="4">
+        <v>863</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="A16" s="4">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>923</v>
+      </c>
+      <c r="M16" t="s">
         <v>10</v>
       </c>
-      <c r="N14">
-        <v>973</v>
-      </c>
-      <c r="O14" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14">
-        <v>1043</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>12</v>
-      </c>
-      <c r="R14">
-        <v>961</v>
-      </c>
-      <c r="S14" t="s">
-        <v>12</v>
-      </c>
-      <c r="T14">
-        <v>969</v>
-      </c>
-      <c r="U14" t="s">
-        <v>24</v>
-      </c>
-      <c r="V14">
-        <v>978</v>
-      </c>
-      <c r="W14" t="s">
-        <v>5</v>
-      </c>
-      <c r="X14">
-        <v>953</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z14">
-        <v>975</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28">
-      <c r="A15">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>970</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15">
-        <v>993</v>
-      </c>
-      <c r="I15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15">
-        <v>999</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5</v>
-      </c>
-      <c r="L15">
-        <v>989</v>
-      </c>
-      <c r="M15" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15">
-        <v>984</v>
-      </c>
-      <c r="O15" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15">
-        <v>1046</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>4</v>
-      </c>
-      <c r="R15">
-        <v>973</v>
-      </c>
-      <c r="S15" t="s">
-        <v>5</v>
-      </c>
-      <c r="T15">
-        <v>986</v>
-      </c>
-      <c r="U15" t="s">
-        <v>8</v>
-      </c>
-      <c r="V15">
-        <v>992</v>
-      </c>
-      <c r="W15" t="s">
-        <v>12</v>
-      </c>
-      <c r="X15">
-        <v>963</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z15">
-        <v>985</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28">
-      <c r="A16">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>1140</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16">
-        <v>1155</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16">
-        <v>1133</v>
-      </c>
-      <c r="M16" t="s">
-        <v>12</v>
-      </c>
       <c r="N16">
-        <v>1136</v>
+        <v>924</v>
       </c>
       <c r="O16" t="s">
         <v>9</v>
       </c>
       <c r="P16">
-        <v>1204</v>
+        <v>992</v>
       </c>
       <c r="Q16" t="s">
         <v>8</v>
       </c>
       <c r="R16">
-        <v>1123</v>
+        <v>909</v>
       </c>
       <c r="S16" t="s">
         <v>8</v>
       </c>
       <c r="T16">
-        <v>1131</v>
+        <v>919</v>
       </c>
       <c r="U16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="V16">
-        <v>1142</v>
+        <v>928</v>
       </c>
       <c r="W16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X16">
-        <v>1119</v>
+        <v>904</v>
       </c>
       <c r="Y16" t="s">
         <v>6</v>
       </c>
       <c r="Z16">
-        <v>1142</v>
+        <v>927</v>
       </c>
       <c r="AA16" t="s">
         <v>10</v>
@@ -2646,266 +2508,404 @@
         <v>13</v>
       </c>
       <c r="F17">
-        <v>1175</v>
+        <v>960</v>
       </c>
       <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>977</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17">
+        <v>993</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17">
+        <v>970</v>
+      </c>
+      <c r="M17" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17">
+        <v>973</v>
+      </c>
+      <c r="O17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <v>1043</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>12</v>
+      </c>
+      <c r="R17">
+        <v>961</v>
+      </c>
+      <c r="S17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T17">
+        <v>969</v>
+      </c>
+      <c r="U17" t="s">
+        <v>24</v>
+      </c>
+      <c r="V17">
+        <v>978</v>
+      </c>
+      <c r="W17" t="s">
+        <v>5</v>
+      </c>
+      <c r="X17">
+        <v>953</v>
+      </c>
+      <c r="Y17" t="s">
         <v>8</v>
       </c>
-      <c r="H17">
-        <v>1194</v>
-      </c>
-      <c r="I17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>1205</v>
-      </c>
-      <c r="K17" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17">
-        <v>1193</v>
-      </c>
-      <c r="M17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N17">
-        <v>1195</v>
-      </c>
-      <c r="O17" t="s">
-        <v>5</v>
-      </c>
-      <c r="P17">
-        <v>1260</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="Z17">
+        <v>975</v>
+      </c>
+      <c r="AA17" t="s">
         <v>10</v>
-      </c>
-      <c r="R17">
-        <v>1181</v>
-      </c>
-      <c r="S17" t="s">
-        <v>10</v>
-      </c>
-      <c r="T17">
-        <v>1195</v>
-      </c>
-      <c r="U17" t="s">
-        <v>25</v>
-      </c>
-      <c r="V17">
-        <v>1200</v>
-      </c>
-      <c r="W17" t="s">
-        <v>11</v>
-      </c>
-      <c r="X17">
-        <v>1172</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z17">
-        <v>1193</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:27">
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="F18">
-        <v>1224</v>
-      </c>
-      <c r="G18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <v>1246</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="T18" t="s">
+        <v>66</v>
+      </c>
+      <c r="U18" t="s">
+        <v>66</v>
+      </c>
+      <c r="V18">
+        <v>983</v>
+      </c>
+      <c r="W18" t="s">
+        <v>62</v>
+      </c>
+      <c r="X18">
+        <v>957</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z18">
+        <v>977</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" s="3">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>970</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>993</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19">
+        <v>999</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>989</v>
+      </c>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19">
+        <v>984</v>
+      </c>
+      <c r="O19" t="s">
         <v>8</v>
       </c>
-      <c r="J18">
-        <v>1255</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="P19">
+        <v>1046</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19">
+        <v>973</v>
+      </c>
+      <c r="S19" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19">
+        <v>986</v>
+      </c>
+      <c r="U19" t="s">
+        <v>8</v>
+      </c>
+      <c r="V19">
+        <v>992</v>
+      </c>
+      <c r="W19" t="s">
+        <v>12</v>
+      </c>
+      <c r="X19">
+        <v>963</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z19">
+        <v>985</v>
+      </c>
+      <c r="AA19" t="s">
         <v>11</v>
       </c>
-      <c r="L18">
-        <v>1234</v>
-      </c>
-      <c r="M18" t="s">
-        <v>6</v>
-      </c>
-      <c r="N18">
-        <v>1233</v>
-      </c>
-      <c r="O18" t="s">
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="4">
+        <v>16</v>
+      </c>
+      <c r="X20" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>1091</v>
+      </c>
+      <c r="AA20" t="s">
         <v>12</v>
-      </c>
-      <c r="P18">
-        <v>1297</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>11</v>
-      </c>
-      <c r="R18">
-        <v>1221</v>
-      </c>
-      <c r="S18" t="s">
-        <v>11</v>
-      </c>
-      <c r="T18">
-        <v>1235</v>
-      </c>
-      <c r="U18" t="s">
-        <v>10</v>
-      </c>
-      <c r="V18">
-        <v>1247</v>
-      </c>
-      <c r="W18" t="s">
-        <v>10</v>
-      </c>
-      <c r="X18">
-        <v>1215</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z18">
-        <v>1242</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
-      <c r="A19">
-        <v>15</v>
-      </c>
-      <c r="T19" t="s">
-        <v>66</v>
-      </c>
-      <c r="U19" t="s">
-        <v>66</v>
-      </c>
-      <c r="V19">
-        <v>629</v>
-      </c>
-      <c r="W19" t="s">
-        <v>63</v>
-      </c>
-      <c r="X19">
-        <v>595</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z19">
-        <v>624</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
-      <c r="A20">
-        <v>16</v>
-      </c>
-      <c r="X20" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z20">
-        <v>824</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:27">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="T21" t="s">
-        <v>66</v>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>1140</v>
+      </c>
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>1155</v>
+      </c>
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21">
+        <v>1133</v>
+      </c>
+      <c r="M21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21">
+        <v>1136</v>
+      </c>
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21">
+        <v>1204</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>8</v>
+      </c>
+      <c r="R21">
+        <v>1123</v>
+      </c>
+      <c r="S21" t="s">
+        <v>8</v>
+      </c>
+      <c r="T21">
+        <v>1131</v>
       </c>
       <c r="U21" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="V21">
-        <v>857</v>
+        <v>1142</v>
       </c>
       <c r="W21" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="X21">
-        <v>826</v>
+        <v>1119</v>
       </c>
       <c r="Y21" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z21">
+        <v>1142</v>
+      </c>
+      <c r="AA21" t="s">
         <v>10</v>
-      </c>
-      <c r="Z21">
-        <v>847</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:27">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="T22" t="s">
-        <v>66</v>
+      <c r="F22">
+        <v>1175</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>1194</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>1205</v>
+      </c>
+      <c r="K22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>1193</v>
+      </c>
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <v>1195</v>
+      </c>
+      <c r="O22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22">
+        <v>1260</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>10</v>
+      </c>
+      <c r="R22">
+        <v>1181</v>
+      </c>
+      <c r="S22" t="s">
+        <v>10</v>
+      </c>
+      <c r="T22">
+        <v>1195</v>
       </c>
       <c r="U22" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="V22">
-        <v>983</v>
+        <v>1200</v>
       </c>
       <c r="W22" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="X22">
-        <v>957</v>
+        <v>1172</v>
       </c>
       <c r="Y22" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Z22">
-        <v>977</v>
+        <v>1193</v>
       </c>
       <c r="AA22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="3">
+        <v>19</v>
+      </c>
+      <c r="F23">
+        <v>1224</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>1246</v>
+      </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>1255</v>
+      </c>
+      <c r="K23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:27">
-      <c r="A23">
-        <v>19</v>
-      </c>
-      <c r="X23" t="s">
-        <v>3</v>
+      <c r="L23">
+        <v>1234</v>
+      </c>
+      <c r="M23" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23">
+        <v>1233</v>
+      </c>
+      <c r="O23" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23">
+        <v>1297</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>11</v>
+      </c>
+      <c r="R23">
+        <v>1221</v>
+      </c>
+      <c r="S23" t="s">
+        <v>11</v>
+      </c>
+      <c r="T23">
+        <v>1235</v>
+      </c>
+      <c r="U23" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23">
+        <v>1247</v>
+      </c>
+      <c r="W23" t="s">
+        <v>10</v>
+      </c>
+      <c r="X23">
+        <v>1215</v>
       </c>
       <c r="Y23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z23">
-        <v>1091</v>
+        <v>1242</v>
       </c>
       <c r="AA23" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:27">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>20</v>
       </c>
       <c r="F24">
@@ -3217,9 +3217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X11" sqref="X11"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4024,7 +4024,7 @@
       <c r="AC15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AD15" s="12" t="s">
+      <c r="AD15" s="14" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4068,130 +4068,130 @@
       <c r="AC16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AD16" s="12"/>
-    </row>
-    <row r="17" spans="1:31" s="13" customFormat="1">
-      <c r="A17" s="13">
+      <c r="AD16" s="14"/>
+    </row>
+    <row r="17" spans="1:31" s="12" customFormat="1">
+      <c r="A17" s="12">
         <v>13</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="R17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="S17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="T17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="U17" s="13" t="s">
+      <c r="U17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="V17" s="13">
+      <c r="V17" s="12">
         <v>1129</v>
       </c>
-      <c r="W17" s="13" t="s">
+      <c r="W17" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="X17" s="13">
+      <c r="X17" s="12">
         <v>1121</v>
       </c>
-      <c r="Y17" s="13" t="s">
+      <c r="Y17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Z17" s="13">
+      <c r="Z17" s="12">
         <v>1135</v>
       </c>
-      <c r="AA17" s="13" t="s">
+      <c r="AA17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AB17" s="13">
+      <c r="AB17" s="12">
         <v>1142</v>
       </c>
-      <c r="AC17" s="13" t="s">
+      <c r="AC17" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AD17" s="14" t="s">
+      <c r="AD17" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:31" s="15" customFormat="1">
-      <c r="A18" s="13">
+    <row r="18" spans="1:31" s="13" customFormat="1">
+      <c r="A18" s="12">
         <v>14</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>1119</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="13">
         <v>1149</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="13">
         <v>1144</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="13">
         <v>1137</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="13">
         <v>1139</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="13">
         <v>1111</v>
       </c>
-      <c r="Q18" s="15" t="s">
+      <c r="Q18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R18" s="15">
+      <c r="R18" s="13">
         <v>1163</v>
       </c>
-      <c r="S18" s="15" t="s">
+      <c r="S18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="15">
+      <c r="T18" s="13">
         <v>1127</v>
       </c>
-      <c r="U18" s="15" t="s">
+      <c r="U18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="V18" s="15">
+      <c r="V18" s="13">
         <v>1143</v>
       </c>
-      <c r="W18" s="15" t="s">
+      <c r="W18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="X18" s="15">
+      <c r="X18" s="13">
         <v>1133</v>
       </c>
-      <c r="Y18" s="15" t="s">
+      <c r="Y18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Z18" s="15">
+      <c r="Z18" s="13">
         <v>1142</v>
       </c>
-      <c r="AA18" s="15" t="s">
+      <c r="AA18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AB18" s="15">
+      <c r="AB18" s="13">
         <v>1139</v>
       </c>
-      <c r="AC18" s="15" t="s">
+      <c r="AC18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="15" t="s">
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="13" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified the crack numbering of AMY
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FBCB9F-D6F9-411D-8C70-795DCD608F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B6E681-3234-4272-B1D6-1A881FB1B135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -19,23 +19,12 @@
     <sheet name="Yellow 6a (broken)" sheetId="2" r:id="rId4"/>
     <sheet name="Green 5 (broken)" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="79">
   <si>
     <t>Y6</t>
   </si>
@@ -286,6 +275,10 @@
   </si>
   <si>
     <t>Same height</t>
+  </si>
+  <si>
+    <t>Same height</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -293,9 +286,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,7 +348,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +376,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,11 +432,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -485,6 +484,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -811,9 +831,9 @@
       <selection pane="topRight" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -858,7 +878,7 @@
       </c>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -906,7 +926,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -968,7 +988,7 @@
       </c>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1030,7 +1050,7 @@
       </c>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1092,7 +1112,7 @@
       </c>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1154,7 +1174,7 @@
       </c>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1218,7 +1238,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1280,7 +1300,7 @@
       </c>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1342,7 +1362,7 @@
       </c>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1404,7 +1424,7 @@
       </c>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1468,7 +1488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1530,7 +1550,7 @@
       </c>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1601,32 +1621,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB24"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="9.25" customWidth="1"/>
-    <col min="4" max="4" width="8.25" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" customWidth="1"/>
+    <col min="3" max="3" width="9.19921875" customWidth="1"/>
+    <col min="4" max="4" width="8.19921875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="9.75" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="13.625" customWidth="1"/>
-    <col min="9" max="10" width="10.25" customWidth="1"/>
-    <col min="11" max="11" width="10.625" customWidth="1"/>
-    <col min="12" max="12" width="11.75" customWidth="1"/>
-    <col min="13" max="13" width="10.25" customWidth="1"/>
-    <col min="14" max="14" width="11.375" customWidth="1"/>
+    <col min="6" max="6" width="9.69921875" customWidth="1"/>
+    <col min="7" max="7" width="10.69921875" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" customWidth="1"/>
+    <col min="9" max="10" width="10.19921875" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="11.69921875" customWidth="1"/>
+    <col min="13" max="13" width="10.19921875" customWidth="1"/>
+    <col min="14" max="14" width="11.3984375" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="1022" width="10.75" customWidth="1"/>
+    <col min="16" max="1022" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
@@ -1643,7 +1665,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1659,8 +1681,8 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1716,8 +1738,8 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:28">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -1725,7 +1747,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
@@ -1761,20 +1783,20 @@
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:28">
-      <c r="A5">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>1</v>
       </c>
       <c r="F5" t="s">
@@ -1844,8 +1866,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
-      <c r="A6">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
       <c r="F6" t="s">
@@ -1915,8 +1937,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
-      <c r="A7" s="3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>3</v>
       </c>
       <c r="B7" s="3"/>
@@ -1990,8 +2012,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="4" customFormat="1">
-      <c r="A8" s="4">
+    <row r="8" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>4</v>
       </c>
       <c r="D8" s="4">
@@ -2070,8 +2092,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
-      <c r="A9">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>5</v>
       </c>
       <c r="T9" t="s">
@@ -2099,8 +2121,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
-      <c r="A10">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>6</v>
       </c>
       <c r="F10" t="s">
@@ -2170,8 +2192,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
-      <c r="A11" s="3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>7</v>
       </c>
       <c r="X11" t="s">
@@ -2187,8 +2209,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
-      <c r="A12" s="4">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>8</v>
       </c>
       <c r="F12">
@@ -2258,108 +2280,112 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="3" customFormat="1">
-      <c r="A13">
+    <row r="13" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
         <v>9</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="F13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="17">
         <v>846</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="17">
         <v>861</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="17">
         <v>842</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="17">
         <v>845</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" s="3">
+      <c r="O13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="17">
         <v>914</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="Q13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="17">
         <v>834</v>
       </c>
-      <c r="S13" s="3" t="s">
+      <c r="S13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13" s="17">
         <v>839</v>
       </c>
-      <c r="U13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="3">
+      <c r="U13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="17">
         <v>849</v>
       </c>
-      <c r="W13" s="3" t="s">
+      <c r="W13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="X13" s="3">
+      <c r="X13" s="17">
         <v>824</v>
       </c>
-      <c r="Y13" s="3" t="s">
+      <c r="Y13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="17">
         <v>846</v>
       </c>
-      <c r="AA13" s="3" t="s">
+      <c r="AA13" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:28">
-      <c r="A14">
+      <c r="AB13" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
         <v>10</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="16">
         <v>857</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="16">
         <v>826</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Y14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="16">
         <v>847</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" s="4" customFormat="1">
-      <c r="A15" s="3">
+      <c r="AB14" s="18"/>
+    </row>
+    <row r="15" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>11</v>
       </c>
       <c r="F15" s="5">
@@ -2432,8 +2458,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
-      <c r="A16" s="4">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>12</v>
       </c>
       <c r="F16" t="s">
@@ -2503,479 +2529,511 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
-      <c r="A17">
+    <row r="17" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>13</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="12">
         <v>960</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="12">
         <v>977</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="12">
         <v>993</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="12">
         <v>970</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="12">
         <v>973</v>
       </c>
-      <c r="O17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P17">
+      <c r="O17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" s="12">
         <v>1043</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="12">
         <v>961</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="12">
         <v>969</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="12">
         <v>978</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="12">
         <v>953</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Y17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="12">
         <v>975</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:27">
-      <c r="A18">
+      <c r="AB17" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22">
         <v>14</v>
       </c>
-      <c r="T18" t="s">
-        <v>66</v>
-      </c>
-      <c r="U18" t="s">
-        <v>66</v>
-      </c>
-      <c r="V18">
+      <c r="F18" s="12">
+        <v>962</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="12">
+        <v>986</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="12">
+        <v>993</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="12">
+        <v>981</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="12">
+        <v>979</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="12">
+        <v>1039</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R18" s="12">
+        <v>966</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="T18" s="12">
+        <v>984</v>
+      </c>
+      <c r="U18" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="V18" s="12">
         <v>983</v>
       </c>
-      <c r="W18" t="s">
+      <c r="W18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="12">
         <v>957</v>
       </c>
-      <c r="Y18" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z18">
+      <c r="Y18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z18" s="12">
         <v>977</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AA18" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:27">
-      <c r="A19" s="3">
+      <c r="AB18" s="15"/>
+    </row>
+    <row r="19" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="F19" s="12">
+        <v>970</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="12">
+        <v>993</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="12">
+        <v>999</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="12">
+        <v>989</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="12">
+        <v>984</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="12">
+        <v>1046</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19" s="12">
+        <v>973</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" s="12">
+        <v>986</v>
+      </c>
+      <c r="U19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="V19" s="12">
+        <v>992</v>
+      </c>
+      <c r="W19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="X19" s="12">
+        <v>963</v>
+      </c>
+      <c r="Y19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z19" s="12">
+        <v>985</v>
+      </c>
+      <c r="AA19" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <v>15</v>
       </c>
-      <c r="F19">
-        <v>970</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>1140</v>
+      </c>
+      <c r="I20" t="s">
         <v>10</v>
       </c>
-      <c r="H19">
-        <v>993</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="J20">
+        <v>1155</v>
+      </c>
+      <c r="K20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20">
+        <v>1133</v>
+      </c>
+      <c r="M20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20">
+        <v>1136</v>
+      </c>
+      <c r="O20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20">
+        <v>1204</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>1123</v>
+      </c>
+      <c r="S20" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20">
+        <v>1131</v>
+      </c>
+      <c r="U20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V20">
+        <v>1142</v>
+      </c>
+      <c r="W20" t="s">
+        <v>4</v>
+      </c>
+      <c r="X20">
+        <v>1119</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z20">
+        <v>1142</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>1175</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>1194</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>1205</v>
+      </c>
+      <c r="K21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21">
+        <v>1193</v>
+      </c>
+      <c r="M21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <v>1195</v>
+      </c>
+      <c r="O21" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>1260</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>10</v>
+      </c>
+      <c r="R21">
+        <v>1181</v>
+      </c>
+      <c r="S21" t="s">
+        <v>10</v>
+      </c>
+      <c r="T21">
+        <v>1195</v>
+      </c>
+      <c r="U21" t="s">
+        <v>25</v>
+      </c>
+      <c r="V21">
+        <v>1200</v>
+      </c>
+      <c r="W21" t="s">
         <v>11</v>
       </c>
-      <c r="J19">
-        <v>999</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="X21">
+        <v>1172</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z21">
+        <v>1193</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>1224</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>1246</v>
+      </c>
+      <c r="I22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22">
+        <v>1255</v>
+      </c>
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>1234</v>
+      </c>
+      <c r="M22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>1233</v>
+      </c>
+      <c r="O22" t="s">
+        <v>12</v>
+      </c>
+      <c r="P22">
+        <v>1297</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22">
+        <v>1221</v>
+      </c>
+      <c r="S22" t="s">
+        <v>11</v>
+      </c>
+      <c r="T22">
+        <v>1235</v>
+      </c>
+      <c r="U22" t="s">
+        <v>10</v>
+      </c>
+      <c r="V22">
+        <v>1247</v>
+      </c>
+      <c r="W22" t="s">
+        <v>10</v>
+      </c>
+      <c r="X22">
+        <v>1215</v>
+      </c>
+      <c r="Y22" t="s">
         <v>5</v>
       </c>
-      <c r="L19">
-        <v>989</v>
-      </c>
-      <c r="M19" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19">
-        <v>984</v>
-      </c>
-      <c r="O19" t="s">
-        <v>8</v>
-      </c>
-      <c r="P19">
-        <v>1046</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>4</v>
-      </c>
-      <c r="R19">
-        <v>973</v>
-      </c>
-      <c r="S19" t="s">
-        <v>5</v>
-      </c>
-      <c r="T19">
-        <v>986</v>
-      </c>
-      <c r="U19" t="s">
-        <v>8</v>
-      </c>
-      <c r="V19">
-        <v>992</v>
-      </c>
-      <c r="W19" t="s">
-        <v>12</v>
-      </c>
-      <c r="X19">
-        <v>963</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z19">
-        <v>985</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
-      <c r="A20" s="4">
-        <v>16</v>
-      </c>
-      <c r="X20" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z20">
-        <v>1091</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>1140</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21">
-        <v>1155</v>
-      </c>
-      <c r="K21" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21">
-        <v>1133</v>
-      </c>
-      <c r="M21" t="s">
-        <v>12</v>
-      </c>
-      <c r="N21">
-        <v>1136</v>
-      </c>
-      <c r="O21" t="s">
-        <v>9</v>
-      </c>
-      <c r="P21">
-        <v>1204</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>8</v>
-      </c>
-      <c r="R21">
-        <v>1123</v>
-      </c>
-      <c r="S21" t="s">
-        <v>8</v>
-      </c>
-      <c r="T21">
-        <v>1131</v>
-      </c>
-      <c r="U21" t="s">
-        <v>9</v>
-      </c>
-      <c r="V21">
-        <v>1142</v>
-      </c>
-      <c r="W21" t="s">
-        <v>4</v>
-      </c>
-      <c r="X21">
-        <v>1119</v>
-      </c>
-      <c r="Y21" t="s">
+      <c r="Z22">
+        <v>1242</v>
+      </c>
+      <c r="AA22" t="s">
         <v>6</v>
       </c>
-      <c r="Z21">
-        <v>1142</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
-      <c r="A22">
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
         <v>18</v>
       </c>
-      <c r="F22">
-        <v>1175</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22">
-        <v>1194</v>
-      </c>
-      <c r="I22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22">
-        <v>1205</v>
-      </c>
-      <c r="K22" t="s">
-        <v>9</v>
-      </c>
-      <c r="L22">
-        <v>1193</v>
-      </c>
-      <c r="M22" t="s">
-        <v>4</v>
-      </c>
-      <c r="N22">
-        <v>1195</v>
-      </c>
-      <c r="O22" t="s">
-        <v>5</v>
-      </c>
-      <c r="P22">
-        <v>1260</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>10</v>
-      </c>
-      <c r="R22">
-        <v>1181</v>
-      </c>
-      <c r="S22" t="s">
-        <v>10</v>
-      </c>
-      <c r="T22">
-        <v>1195</v>
-      </c>
-      <c r="U22" t="s">
-        <v>25</v>
-      </c>
-      <c r="V22">
-        <v>1200</v>
-      </c>
-      <c r="W22" t="s">
-        <v>11</v>
-      </c>
-      <c r="X22">
-        <v>1172</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z22">
-        <v>1193</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
-      <c r="A23" s="3">
-        <v>19</v>
-      </c>
       <c r="F23">
-        <v>1224</v>
+        <v>1356</v>
       </c>
       <c r="G23" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="H23">
-        <v>1246</v>
+        <v>1381</v>
       </c>
       <c r="I23" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="J23">
-        <v>1255</v>
+        <v>1387</v>
       </c>
       <c r="K23" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="L23">
-        <v>1234</v>
+        <v>1373</v>
       </c>
       <c r="M23" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="N23">
-        <v>1233</v>
+        <v>1370</v>
       </c>
       <c r="O23" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="P23">
-        <v>1297</v>
+        <v>1431</v>
       </c>
       <c r="Q23" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="R23">
-        <v>1221</v>
+        <v>1358</v>
       </c>
       <c r="S23" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="T23">
-        <v>1235</v>
+        <v>1374</v>
       </c>
       <c r="U23" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="V23">
-        <v>1247</v>
+        <v>1384</v>
       </c>
       <c r="W23" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="X23">
-        <v>1215</v>
+        <v>1351</v>
       </c>
       <c r="Y23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z23">
-        <v>1242</v>
+        <v>1378</v>
       </c>
       <c r="AA23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
-      <c r="A24" s="4">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <v>1356</v>
-      </c>
-      <c r="G24" t="s">
-        <v>59</v>
-      </c>
-      <c r="H24">
-        <v>1381</v>
-      </c>
-      <c r="I24" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24">
-        <v>1387</v>
-      </c>
-      <c r="K24" t="s">
-        <v>58</v>
-      </c>
-      <c r="L24">
-        <v>1373</v>
-      </c>
-      <c r="M24" t="s">
-        <v>60</v>
-      </c>
-      <c r="N24">
-        <v>1370</v>
-      </c>
-      <c r="O24" t="s">
-        <v>61</v>
-      </c>
-      <c r="P24">
-        <v>1431</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>58</v>
-      </c>
-      <c r="R24">
-        <v>1358</v>
-      </c>
-      <c r="S24" t="s">
-        <v>58</v>
-      </c>
-      <c r="T24">
-        <v>1374</v>
-      </c>
-      <c r="U24" t="s">
-        <v>62</v>
-      </c>
-      <c r="V24">
-        <v>1384</v>
-      </c>
-      <c r="W24" t="s">
-        <v>62</v>
-      </c>
-      <c r="X24">
-        <v>1351</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z24">
-        <v>1378</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="A18:A19"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39416666666666667" bottom="0.39416666666666667" header="0" footer="0"/>
   <headerFooter>
@@ -2993,17 +3051,17 @@
       <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="10.75" customWidth="1"/>
+    <col min="1" max="1024" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -3060,7 +3118,7 @@
       </c>
       <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -3117,7 +3175,7 @@
       </c>
       <c r="AA4" s="6"/>
     </row>
-    <row r="5" spans="1:28" s="4" customFormat="1">
+    <row r="5" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -3217,26 +3275,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="10.75" customWidth="1"/>
-    <col min="17" max="17" width="12.25" customWidth="1"/>
-    <col min="18" max="29" width="10.75" customWidth="1"/>
-    <col min="30" max="30" width="11.875" customWidth="1"/>
-    <col min="31" max="1024" width="10.75" customWidth="1"/>
+    <col min="1" max="16" width="10.69921875" customWidth="1"/>
+    <col min="17" max="17" width="12.19921875" customWidth="1"/>
+    <col min="18" max="29" width="10.69921875" customWidth="1"/>
+    <col min="30" max="30" width="11.8984375" customWidth="1"/>
+    <col min="31" max="1024" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3297,7 +3355,7 @@
       </c>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3358,7 +3416,7 @@
       </c>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3435,7 +3493,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3512,7 +3570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1">
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3553,7 +3611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3594,7 +3652,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3629,7 +3687,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3706,7 +3764,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3783,7 +3841,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3824,7 +3882,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3901,7 +3959,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3978,7 +4036,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="10" customFormat="1">
+    <row r="15" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>11</v>
       </c>
@@ -4028,7 +4086,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="10" customFormat="1">
+    <row r="16" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>12</v>
       </c>
@@ -4070,7 +4128,7 @@
       </c>
       <c r="AD16" s="14"/>
     </row>
-    <row r="17" spans="1:31" s="12" customFormat="1">
+    <row r="17" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>13</v>
       </c>
@@ -4114,7 +4172,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:31" s="13" customFormat="1">
+    <row r="18" spans="1:31" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>14</v>
       </c>
@@ -4195,7 +4253,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -4272,7 +4330,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -4349,7 +4407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -4396,7 +4454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -4473,7 +4531,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -4514,7 +4572,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:31" s="3" customFormat="1">
+    <row r="24" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -4615,17 +4673,17 @@
       <selection pane="topRight" activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="10.75" customWidth="1"/>
+    <col min="1" max="1024" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -4702,7 +4760,7 @@
       </c>
       <c r="AK3" s="6"/>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -4779,7 +4837,7 @@
       </c>
       <c r="AK4" s="6"/>
     </row>
-    <row r="5" spans="1:37" s="4" customFormat="1">
+    <row r="5" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -4883,7 +4941,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4930,7 +4988,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -4977,7 +5035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:37" s="7" customFormat="1">
+    <row r="8" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -5042,7 +5100,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:37" s="8" customFormat="1">
+    <row r="9" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5077,7 +5135,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:37" s="8" customFormat="1">
+    <row r="10" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5118,7 +5176,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:37" s="8" customFormat="1">
+    <row r="11" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -5183,7 +5241,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:37" s="7" customFormat="1">
+    <row r="12" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -5251,7 +5309,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:37" s="8" customFormat="1">
+    <row r="13" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
modified the crack site recording for first dose 2nd specimen
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B6E681-3234-4272-B1D6-1A881FB1B135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2FE5FF-0F8E-4BE0-B721-7AD3048B945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="1440" windowWidth="12972" windowHeight="8856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="79">
   <si>
     <t>Y6</t>
   </si>
@@ -479,20 +479,11 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -503,8 +494,17 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -826,9 +826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28D44DB-860F-414F-BC56-ABC9B4ED1201}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1094,11 +1094,11 @@
       <c r="Q5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="3" t="s">
-        <v>3</v>
+      <c r="R5" s="3">
+        <v>617</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="T5" s="3">
         <v>624</v>
@@ -1615,7 +1615,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1623,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
@@ -1648,7 +1648,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
@@ -1682,7 +1682,7 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1739,7 +1739,7 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -2280,109 +2280,109 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+    <row r="13" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>9</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="17">
+      <c r="F13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15">
         <v>846</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="15">
         <v>861</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="15">
         <v>842</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="15">
         <v>845</v>
       </c>
-      <c r="O13" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="15">
         <v>914</v>
       </c>
-      <c r="Q13" s="17" t="s">
+      <c r="Q13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="17">
+      <c r="R13" s="15">
         <v>834</v>
       </c>
-      <c r="S13" s="17" t="s">
+      <c r="S13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T13" s="17">
+      <c r="T13" s="15">
         <v>839</v>
       </c>
-      <c r="U13" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="17">
+      <c r="U13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="15">
         <v>849</v>
       </c>
-      <c r="W13" s="17" t="s">
+      <c r="W13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="X13" s="17">
+      <c r="X13" s="15">
         <v>824</v>
       </c>
-      <c r="Y13" s="17" t="s">
+      <c r="Y13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Z13" s="17">
+      <c r="Z13" s="15">
         <v>846</v>
       </c>
-      <c r="AA13" s="17" t="s">
+      <c r="AA13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="AB13" s="18" t="s">
+      <c r="AB13" s="19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+    <row r="14" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <v>10</v>
       </c>
-      <c r="T14" s="16" t="s">
+      <c r="T14" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="U14" s="16" t="s">
+      <c r="U14" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="V14" s="16">
+      <c r="V14" s="14">
         <v>857</v>
       </c>
-      <c r="W14" s="16" t="s">
+      <c r="W14" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="X14" s="16">
+      <c r="X14" s="14">
         <v>826</v>
       </c>
-      <c r="Y14" s="16" t="s">
+      <c r="Y14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Z14" s="16">
+      <c r="Z14" s="14">
         <v>847</v>
       </c>
-      <c r="AA14" s="16" t="s">
+      <c r="AA14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AB14" s="18"/>
+      <c r="AB14" s="19"/>
     </row>
     <row r="15" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -2530,7 +2530,7 @@
       </c>
     </row>
     <row r="17" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="18">
         <v>13</v>
       </c>
       <c r="F17" s="12">
@@ -2599,12 +2599,12 @@
       <c r="AA17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AB17" s="15" t="s">
+      <c r="AB17" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="A18" s="21">
         <v>14</v>
       </c>
       <c r="F18" s="12">
@@ -2673,10 +2673,10 @@
       <c r="AA18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AB18" s="15"/>
+      <c r="AB18" s="20"/>
     </row>
     <row r="19" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="21"/>
       <c r="F19" s="12">
         <v>970</v>
       </c>
@@ -4082,7 +4082,7 @@
       <c r="AC15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AD15" s="14" t="s">
+      <c r="AD15" s="22" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4126,7 +4126,7 @@
       <c r="AC16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AD16" s="14"/>
+      <c r="AD16" s="22"/>
     </row>
     <row r="17" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -4168,7 +4168,7 @@
       <c r="AC17" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AD17" s="15" t="s">
+      <c r="AD17" s="20" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4248,7 +4248,7 @@
       <c r="AC18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="AD18" s="15"/>
+      <c r="AD18" s="20"/>
       <c r="AE18" s="13" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
modified the recording, added some not-easy-to-tell cracks
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2FE5FF-0F8E-4BE0-B721-7AD3048B945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82897690-71D6-4391-85C6-84D59D19A8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="1440" windowWidth="12972" windowHeight="8856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="80">
   <si>
     <t>Y6</t>
   </si>
@@ -278,6 +278,10 @@
   </si>
   <si>
     <t>Same height</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>left (same height as crack8)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -826,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28D44DB-860F-414F-BC56-ABC9B4ED1201}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F7" sqref="F7"/>
     </sheetView>
@@ -1623,9 +1627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2196,11 +2200,11 @@
       <c r="A11" s="8">
         <v>7</v>
       </c>
-      <c r="X11" t="s">
-        <v>3</v>
+      <c r="X11">
+        <v>800</v>
       </c>
       <c r="Y11" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="Z11">
         <v>824</v>

</xml_diff>

<commit_message>
measured the crack growth of AMY6 (part)
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\_fatigue3D_AM_imagebased_exp\fatigue_crack_tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82897690-71D6-4391-85C6-84D59D19A8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE4668A-1E89-4036-8B9E-43109D0F99C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39405" yWindow="330" windowWidth="14535" windowHeight="15135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -19,12 +19,23 @@
     <sheet name="Yellow 6a (broken)" sheetId="2" r:id="rId4"/>
     <sheet name="Green 5 (broken)" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="80">
   <si>
     <t>Y6</t>
   </si>
@@ -290,9 +301,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,7 +447,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -835,9 +846,9 @@
       <selection pane="topRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -882,7 +893,7 @@
       </c>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -930,7 +941,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -992,7 +1003,7 @@
       </c>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1054,7 +1065,7 @@
       </c>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1116,7 +1127,7 @@
       </c>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1178,7 +1189,7 @@
       </c>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1242,7 +1253,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1304,7 +1315,7 @@
       </c>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1366,7 +1377,7 @@
       </c>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1428,7 +1439,7 @@
       </c>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1492,7 +1503,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1554,7 +1565,7 @@
       </c>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1628,30 +1639,32 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.69921875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.69921875" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="4" max="4" width="8.19921875" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="9.69921875" customWidth="1"/>
-    <col min="7" max="7" width="10.69921875" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
-    <col min="9" max="10" width="10.19921875" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" customWidth="1"/>
-    <col min="12" max="12" width="11.69921875" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="10" width="10.25" customWidth="1"/>
+    <col min="11" max="11" width="10.625" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="10.25" customWidth="1"/>
+    <col min="14" max="14" width="11.375" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="1022" width="10.69921875" customWidth="1"/>
+    <col min="16" max="24" width="10.75" customWidth="1"/>
+    <col min="25" max="25" width="23.125" customWidth="1"/>
+    <col min="26" max="1022" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1682,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1685,7 +1698,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -1742,7 +1755,7 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -1799,7 +1812,7 @@
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1870,7 +1883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1941,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -2016,7 +2029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" s="4" customFormat="1">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -2096,7 +2109,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -2125,7 +2138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -2196,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="8">
         <v>7</v>
       </c>
@@ -2213,7 +2226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="8">
         <v>8</v>
       </c>
@@ -2284,7 +2297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="15" customFormat="1">
       <c r="A13" s="17">
         <v>9</v>
       </c>
@@ -2358,7 +2371,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="14" customFormat="1">
       <c r="A14" s="17">
         <v>10</v>
       </c>
@@ -2388,7 +2401,7 @@
       </c>
       <c r="AB14" s="19"/>
     </row>
-    <row r="15" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="4" customFormat="1">
       <c r="A15" s="8">
         <v>11</v>
       </c>
@@ -2462,7 +2475,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="8">
         <v>12</v>
       </c>
@@ -2533,7 +2546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="12" customFormat="1">
       <c r="A17" s="18">
         <v>13</v>
       </c>
@@ -2607,7 +2620,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="12" customFormat="1">
       <c r="A18" s="21">
         <v>14</v>
       </c>
@@ -2679,7 +2692,7 @@
       </c>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="12" customFormat="1">
       <c r="A19" s="21"/>
       <c r="F19" s="12">
         <v>970</v>
@@ -2748,7 +2761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -2819,7 +2832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -2890,7 +2903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -2961,7 +2974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -3055,17 +3068,17 @@
       <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -3122,7 +3135,7 @@
       </c>
       <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -3179,7 +3192,7 @@
       </c>
       <c r="AA4" s="6"/>
     </row>
-    <row r="5" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="4" customFormat="1">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -3279,26 +3292,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16" width="10.69921875" customWidth="1"/>
-    <col min="17" max="17" width="12.19921875" customWidth="1"/>
-    <col min="18" max="29" width="10.69921875" customWidth="1"/>
-    <col min="30" max="30" width="11.8984375" customWidth="1"/>
-    <col min="31" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="16" width="10.75" customWidth="1"/>
+    <col min="17" max="17" width="12.25" customWidth="1"/>
+    <col min="18" max="29" width="10.75" customWidth="1"/>
+    <col min="30" max="30" width="11.875" customWidth="1"/>
+    <col min="31" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3359,7 +3372,7 @@
       </c>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3420,7 +3433,7 @@
       </c>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3497,7 +3510,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3574,7 +3587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="3" customFormat="1">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3615,7 +3628,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3656,7 +3669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3691,7 +3704,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3768,7 +3781,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3845,7 +3858,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3886,7 +3899,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3963,7 +3976,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>10</v>
       </c>
@@ -4040,7 +4053,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="10" customFormat="1">
       <c r="A15" s="10">
         <v>11</v>
       </c>
@@ -4090,7 +4103,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="10" customFormat="1">
       <c r="A16" s="10">
         <v>12</v>
       </c>
@@ -4132,7 +4145,7 @@
       </c>
       <c r="AD16" s="22"/>
     </row>
-    <row r="17" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" s="12" customFormat="1">
       <c r="A17" s="12">
         <v>13</v>
       </c>
@@ -4176,7 +4189,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:31" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" s="13" customFormat="1">
       <c r="A18" s="12">
         <v>14</v>
       </c>
@@ -4257,7 +4270,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19">
         <v>15</v>
       </c>
@@ -4334,7 +4347,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20">
         <v>16</v>
       </c>
@@ -4411,7 +4424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21">
         <v>17</v>
       </c>
@@ -4458,7 +4471,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22">
         <v>18</v>
       </c>
@@ -4535,7 +4548,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23">
         <v>19</v>
       </c>
@@ -4576,7 +4589,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" s="3" customFormat="1">
       <c r="A24">
         <v>20</v>
       </c>
@@ -4670,24 +4683,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AK13"/>
+  <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ13" sqref="AJ13"/>
+      <selection pane="topRight" activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1024" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1024" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -4764,7 +4777,7 @@
       </c>
       <c r="AK3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -4801,39 +4814,39 @@
       </c>
       <c r="Q4" s="6"/>
       <c r="R4" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W4" s="6"/>
       <c r="X4" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6" t="s">
@@ -4841,7 +4854,7 @@
       </c>
       <c r="AK4" s="6"/>
     </row>
-    <row r="5" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" s="4" customFormat="1">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -4945,7 +4958,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4992,7 +5005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5039,7 +5052,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" s="7" customFormat="1">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -5104,7 +5117,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" s="8" customFormat="1">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5139,7 +5152,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" s="8" customFormat="1">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5180,33 +5193,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" s="8" customFormat="1">
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="V11" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="W11" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="R11" s="8">
-        <v>1203</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T11" s="8">
-        <v>1232</v>
-      </c>
-      <c r="U11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="V11" s="8">
-        <v>1233</v>
-      </c>
-      <c r="W11" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="X11" s="8">
         <v>1205</v>
@@ -5245,7 +5240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" s="7" customFormat="1">
       <c r="A12">
         <v>8</v>
       </c>
@@ -5311,59 +5306,6 @@
       </c>
       <c r="AJ12" s="7" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="T13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="U13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="V13" s="8">
-        <v>1456</v>
-      </c>
-      <c r="W13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="X13" s="8">
-        <v>1416</v>
-      </c>
-      <c r="Y13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z13" s="8">
-        <v>1424</v>
-      </c>
-      <c r="AA13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB13" s="8">
-        <v>1432</v>
-      </c>
-      <c r="AC13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD13" s="8">
-        <v>1439</v>
-      </c>
-      <c r="AE13" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF13" s="8">
-        <v>1429</v>
-      </c>
-      <c r="AG13" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH13" s="8">
-        <v>1448</v>
-      </c>
-      <c r="AI13" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished the measure of all crack geometry
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE4668A-1E89-4036-8B9E-43109D0F99C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE4C15-7E1A-43F2-86F3-266F25C81E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39405" yWindow="330" windowWidth="14535" windowHeight="15135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40980" yWindow="1470" windowWidth="11115" windowHeight="11205" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="80">
   <si>
     <t>Y6</t>
   </si>
@@ -1638,9 +1638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3292,9 +3292,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3785,35 +3785,11 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="F11">
-        <v>804</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>817</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>824</v>
-      </c>
-      <c r="K11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11">
-        <v>824</v>
-      </c>
-      <c r="M11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11">
-        <v>829</v>
+      <c r="N11" t="s">
+        <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="P11">
         <v>780</v>

</xml_diff>

<commit_message>
renewed the combined cracks folder
</commit_message>
<xml_diff>
--- a/crack_site_recording.xlsx
+++ b/crack_site_recording.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Research\AM_fatigue\fatigue-crack-tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox (ASU)\Research\Image based AM fatigue analysis\fatigue-crack-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE4C15-7E1A-43F2-86F3-266F25C81E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9C19B1-87AE-4986-9FB7-B864443D0753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40980" yWindow="1470" windowWidth="11115" windowHeight="11205" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32550" yWindow="1725" windowWidth="18060" windowHeight="11205" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS2 (broken)" sheetId="5" r:id="rId1"/>
@@ -3292,9 +3292,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E27" sqref="E27:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4661,9 +4661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD15" sqref="AD15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>